<commit_message>
added example for image files detection
</commit_message>
<xml_diff>
--- a/DesignNote.xlsx
+++ b/DesignNote.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a59c1bdb761853cd/masksDetection/masksDetection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="11_F25DC773A252ABDACC1048E0995B61245BDE58ED" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{45622070-91A6-4D32-9D0B-6FD789E23BD3}"/>
+  <xr:revisionPtr revIDLastSave="211" documentId="11_F25DC773A252ABDACC1048E0995B61245BDE58ED" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{53117C9E-5E9E-4CBA-A076-AF4AC134A97B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="History" sheetId="2" r:id="rId1"/>
     <sheet name="system diagrams" sheetId="1" r:id="rId2"/>
+    <sheet name="facesamples" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>20200428_0</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -37,6 +38,26 @@
   </si>
   <si>
     <t>T.I.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20200502_0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Added sheet "facesamples"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20200505_0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modified the sheet "system diagram"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20200506_0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -108,6 +129,65 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>189243</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>193448</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>28471</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="64" name="圖片 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{106D9965-0441-4778-A558-BA250CCC761A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="10059" t="11184"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11553092" y="11021366"/>
+          <a:ext cx="3516941" cy="1966967"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
@@ -134,8 +214,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6502094" y="3257204"/>
-          <a:ext cx="2709792" cy="1357745"/>
+          <a:off x="6393237" y="3288872"/>
+          <a:ext cx="2660311" cy="1371599"/>
           <a:chOff x="1760220" y="1402080"/>
           <a:chExt cx="2682240" cy="1333500"/>
         </a:xfrm>
@@ -261,8 +341,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6031110" y="1667397"/>
-          <a:ext cx="1823833" cy="931718"/>
+          <a:off x="5932149" y="1683231"/>
+          <a:ext cx="1784249" cy="941614"/>
           <a:chOff x="7041246" y="1945791"/>
           <a:chExt cx="1801991" cy="914400"/>
         </a:xfrm>
@@ -281,13 +361,13 @@
           </xdr:cNvPicPr>
         </xdr:nvPicPr>
         <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
             <a:extLst>
               <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
                 <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
               </a:ext>
               <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
               </a:ext>
             </a:extLst>
           </a:blip>
@@ -389,8 +469,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7793182" y="1690255"/>
-          <a:ext cx="3151743" cy="931718"/>
+          <a:off x="7654637" y="1706089"/>
+          <a:ext cx="3102262" cy="941614"/>
           <a:chOff x="7680960" y="1905000"/>
           <a:chExt cx="3116543" cy="914400"/>
         </a:xfrm>
@@ -409,13 +489,13 @@
           </xdr:cNvPicPr>
         </xdr:nvPicPr>
         <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
             <a:extLst>
               <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
                 <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
               </a:ext>
               <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
               </a:ext>
             </a:extLst>
           </a:blip>
@@ -512,13 +592,13 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
             <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId5"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -565,13 +645,13 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
             <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId6"/>
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId7"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -751,13 +831,13 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
             <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId8"/>
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId9"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -804,13 +884,13 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
             <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId6"/>
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId7"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1526,6 +1606,1898 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>32022</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>51953</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>525087</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>51952</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="29" name="群組 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B5FCD9C-FECB-410E-B782-D432FD2AB41C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="6563451" y="11808524"/>
+          <a:ext cx="2670207" cy="1371599"/>
+          <a:chOff x="1760220" y="1402080"/>
+          <a:chExt cx="2682240" cy="1333500"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="34" name="矩形 33">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5821644C-A19C-4249-BDC0-8842D16F9C38}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1760220" y="1402080"/>
+            <a:ext cx="2682240" cy="1333500"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="41" name="文字方塊 40">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE9AF776-236D-4948-9AC4-727AD36A3B68}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1868403" y="1736815"/>
+            <a:ext cx="1459961" cy="333264"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW" sz="1600" b="1"/>
+              <a:t>image_AI_0.py</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1600" b="1"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>115220</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>13855</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>276508</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>169718</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="42" name="群組 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEC0F77F-AAE2-4273-A17D-225F167B1812}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="6102363" y="10202884"/>
+          <a:ext cx="1794145" cy="939634"/>
+          <a:chOff x="7041246" y="1945791"/>
+          <a:chExt cx="1801991" cy="914400"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="43" name="圖形 42" descr="宣紙">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD5D5BDC-B37A-45D8-8FC0-8A1BCDB80C56}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7626206" y="1945791"/>
+            <a:ext cx="914400" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="44" name="文字方塊 43">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C41799E-3080-49EA-BEBB-B1EF2E0DB13F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7041246" y="1995675"/>
+            <a:ext cx="1801991" cy="828011"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW" sz="2400" b="1"/>
+              <a:t>.H5</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW" sz="2400" b="1"/>
+              <a:t>(Yolo model)</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-TW" altLang="en-US" sz="2400" b="1"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>214747</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>36713</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>41399</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>192576</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="45" name="群組 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D8F2ABA-5C2A-4EB6-9A73-A341C30D7BF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="7834747" y="10225742"/>
+          <a:ext cx="3092366" cy="939634"/>
+          <a:chOff x="7680960" y="1905000"/>
+          <a:chExt cx="3116543" cy="914400"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="46" name="圖形 45" descr="宣紙">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4060F03-D018-47BE-AE63-797340B4D819}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7680960" y="1905000"/>
+            <a:ext cx="914400" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="47" name="文字方塊 46">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED8D7D2F-0F36-4C75-AA8A-B1F8A46B6A3A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7795260" y="2308860"/>
+            <a:ext cx="3002243" cy="459314"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW" sz="2400" b="1"/>
+              <a:t>.detection_config.json</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-TW" altLang="en-US" sz="2400" b="1"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>429492</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>50569</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1872051" cy="468013"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="文字方塊 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F03767A-C9EE-4895-A833-350525CEDBC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2606635" y="10631483"/>
+          <a:ext cx="1872051" cy="468013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="2400"/>
+            <a:t>Source</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="2400" baseline="0"/>
+            <a:t> image</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>332510</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>50567</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>415637</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>64421</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="直線單箭頭接點 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEB753C2-F7F7-4A87-BFD0-432CD1E00CCC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5874328" y="12270276"/>
+          <a:ext cx="637309" cy="13854"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="50800">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>263237</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>105985</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>346364</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>119839</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="57" name="直線單箭頭接點 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B4FF4A1-F80D-471B-BCEE-811AFC4BACB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9684328" y="12325694"/>
+          <a:ext cx="637309" cy="13854"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="50800">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>124691</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>50567</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>124692</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>119839</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="58" name="直線單箭頭接點 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23EE579D-45AF-4F66-BFC3-9102AB4089B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8437418" y="11106494"/>
+          <a:ext cx="1" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="50800">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>166254</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>36713</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>166255</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>105985</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="59" name="直線單箭頭接點 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19BED790-20A7-445D-8936-DC5917A40655}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7370618" y="11092640"/>
+          <a:ext cx="1" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="50800">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>110837</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>175258</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1005468" cy="843693"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="文字方塊 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D317BBC1-91CE-4DA2-9951-5C67BCFDBA0D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9531928" y="12588931"/>
+          <a:ext cx="1005468" cy="843693"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="2400"/>
+            <a:t>result</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="2400"/>
+            <a:t>export</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>236317</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>27708</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>41564</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>47581</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="62" name="圖片 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D96CD34-2231-468A-8B9B-056B071421CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2453044" y="11471563"/>
+          <a:ext cx="3130338" cy="1765545"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>99000</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>166255</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>27709</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>166254</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="圖形 51" descr="電視">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11F1B13B-30A2-4EA8-B67D-3381C2072837}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11182636" y="10640291"/>
+          <a:ext cx="4362164" cy="3103418"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 172316 w 2642177"/>
+            <a:gd name="connsiteY0" fmla="*/ 1506898 h 1970559"/>
+            <a:gd name="connsiteX1" fmla="*/ 172316 w 2642177"/>
+            <a:gd name="connsiteY1" fmla="*/ 173873 h 1970559"/>
+            <a:gd name="connsiteX2" fmla="*/ 2469862 w 2642177"/>
+            <a:gd name="connsiteY2" fmla="*/ 173873 h 1970559"/>
+            <a:gd name="connsiteX3" fmla="*/ 2469862 w 2642177"/>
+            <a:gd name="connsiteY3" fmla="*/ 1506898 h 1970559"/>
+            <a:gd name="connsiteX4" fmla="*/ 172316 w 2642177"/>
+            <a:gd name="connsiteY4" fmla="*/ 1506898 h 1970559"/>
+            <a:gd name="connsiteX5" fmla="*/ 1550844 w 2642177"/>
+            <a:gd name="connsiteY5" fmla="*/ 1854644 h 1970559"/>
+            <a:gd name="connsiteX6" fmla="*/ 1091334 w 2642177"/>
+            <a:gd name="connsiteY6" fmla="*/ 1854644 h 1970559"/>
+            <a:gd name="connsiteX7" fmla="*/ 1091334 w 2642177"/>
+            <a:gd name="connsiteY7" fmla="*/ 1680771 h 1970559"/>
+            <a:gd name="connsiteX8" fmla="*/ 1550844 w 2642177"/>
+            <a:gd name="connsiteY8" fmla="*/ 1680771 h 1970559"/>
+            <a:gd name="connsiteX9" fmla="*/ 1550844 w 2642177"/>
+            <a:gd name="connsiteY9" fmla="*/ 1854644 h 1970559"/>
+            <a:gd name="connsiteX10" fmla="*/ 2642178 w 2642177"/>
+            <a:gd name="connsiteY10" fmla="*/ 1680771 h 1970559"/>
+            <a:gd name="connsiteX11" fmla="*/ 2642178 w 2642177"/>
+            <a:gd name="connsiteY11" fmla="*/ 0 h 1970559"/>
+            <a:gd name="connsiteX12" fmla="*/ 0 w 2642177"/>
+            <a:gd name="connsiteY12" fmla="*/ 0 h 1970559"/>
+            <a:gd name="connsiteX13" fmla="*/ 0 w 2642177"/>
+            <a:gd name="connsiteY13" fmla="*/ 1680771 h 1970559"/>
+            <a:gd name="connsiteX14" fmla="*/ 919018 w 2642177"/>
+            <a:gd name="connsiteY14" fmla="*/ 1680771 h 1970559"/>
+            <a:gd name="connsiteX15" fmla="*/ 919018 w 2642177"/>
+            <a:gd name="connsiteY15" fmla="*/ 1854644 h 1970559"/>
+            <a:gd name="connsiteX16" fmla="*/ 402071 w 2642177"/>
+            <a:gd name="connsiteY16" fmla="*/ 1854644 h 1970559"/>
+            <a:gd name="connsiteX17" fmla="*/ 344632 w 2642177"/>
+            <a:gd name="connsiteY17" fmla="*/ 1912602 h 1970559"/>
+            <a:gd name="connsiteX18" fmla="*/ 344632 w 2642177"/>
+            <a:gd name="connsiteY18" fmla="*/ 1970559 h 1970559"/>
+            <a:gd name="connsiteX19" fmla="*/ 2297546 w 2642177"/>
+            <a:gd name="connsiteY19" fmla="*/ 1970559 h 1970559"/>
+            <a:gd name="connsiteX20" fmla="*/ 2297546 w 2642177"/>
+            <a:gd name="connsiteY20" fmla="*/ 1912602 h 1970559"/>
+            <a:gd name="connsiteX21" fmla="*/ 2240107 w 2642177"/>
+            <a:gd name="connsiteY21" fmla="*/ 1854644 h 1970559"/>
+            <a:gd name="connsiteX22" fmla="*/ 1723159 w 2642177"/>
+            <a:gd name="connsiteY22" fmla="*/ 1854644 h 1970559"/>
+            <a:gd name="connsiteX23" fmla="*/ 1723159 w 2642177"/>
+            <a:gd name="connsiteY23" fmla="*/ 1680771 h 1970559"/>
+            <a:gd name="connsiteX24" fmla="*/ 2642178 w 2642177"/>
+            <a:gd name="connsiteY24" fmla="*/ 1680771 h 1970559"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX8" y="connsiteY8"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX9" y="connsiteY9"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX10" y="connsiteY10"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX11" y="connsiteY11"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX12" y="connsiteY12"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX13" y="connsiteY13"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX14" y="connsiteY14"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX15" y="connsiteY15"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX16" y="connsiteY16"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX17" y="connsiteY17"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX18" y="connsiteY18"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX19" y="connsiteY19"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX20" y="connsiteY20"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX21" y="connsiteY21"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX22" y="connsiteY22"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX23" y="connsiteY23"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX24" y="connsiteY24"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="2642177" h="1970559">
+              <a:moveTo>
+                <a:pt x="172316" y="1506898"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="172316" y="173873"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="2469862" y="173873"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="2469862" y="1506898"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="172316" y="1506898"/>
+              </a:lnTo>
+              <a:close/>
+              <a:moveTo>
+                <a:pt x="1550844" y="1854644"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="1091334" y="1854644"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1091334" y="1680771"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1550844" y="1680771"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1550844" y="1854644"/>
+              </a:lnTo>
+              <a:close/>
+              <a:moveTo>
+                <a:pt x="2642178" y="1680771"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="2642178" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="1680771"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="919018" y="1680771"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="919018" y="1854644"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="402071" y="1854644"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="370479" y="1854644"/>
+                <a:pt x="344632" y="1880725"/>
+                <a:pt x="344632" y="1912602"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="344632" y="1970559"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="2297546" y="1970559"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="2297546" y="1912602"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="2297546" y="1880725"/>
+                <a:pt x="2271699" y="1854644"/>
+                <a:pt x="2240107" y="1854644"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="1723159" y="1854644"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1723159" y="1680771"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="2642178" y="1680771"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="000000"/>
+        </a:solidFill>
+        <a:ln w="28674" cap="flat">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>349563</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>41564</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>105508</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>82061</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="矩形 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0F5FF55-6860-42CE-A619-6FACE808527C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11920240" y="11647410"/>
+          <a:ext cx="306930" cy="233928"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>198227</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>154531</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>463061</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>17585</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="矩形 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CAA13F3-2596-4052-B91B-05A7792F7CAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12319889" y="11566946"/>
+          <a:ext cx="264834" cy="249916"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>394321</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>99646</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>255776</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>98100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="矩形 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F33DCCAD-2665-42CA-B63B-F65E2C026B41}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13617952" y="11512061"/>
+          <a:ext cx="412439" cy="385316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>222739</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>78332</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>84193</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>76254</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="矩形 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E20D5C5-C433-4952-91CC-9C07951C015C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14548339" y="11490747"/>
+          <a:ext cx="412439" cy="384784"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>418833</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>87923</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>280287</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>85845</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="68" name="矩形 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA016AB1-1C3D-4DFB-A04B-08A08004D838}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13091479" y="11500338"/>
+          <a:ext cx="412439" cy="384784"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>337456</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>152398</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2248629" cy="468013"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="文字方塊 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C62C1D20-C50B-46B5-82EB-5E47A15102AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12311742" y="9949541"/>
+          <a:ext cx="2248629" cy="468013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="2400">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Wearning</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="2400" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> masks</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="2400">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>174172</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>141514</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>97972</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>32657</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="直線單箭頭接點 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBB22945-DBAE-456E-B188-CC0514777AD7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13237029" y="10330543"/>
+          <a:ext cx="468086" cy="1262743"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>332014</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>11974</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3246979" cy="468013"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="文字方塊 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70404B2C-A64D-4ED1-B1FB-4931B0B0C6CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10129157" y="14119860"/>
+          <a:ext cx="3246979" cy="468013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="2400" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>without w</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="2400">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>earning</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="2400" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> masks</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="2400">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>322647</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>11974</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="71" name="直線單箭頭接點 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23663C2A-CDE9-4678-AABC-8FC62526BBF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="70" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11752647" y="11975374"/>
+          <a:ext cx="526439" cy="2144486"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>242346</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>78023</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="圖片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA28A199-8338-4752-ADE9-1A9B2DEDD621}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1339626" y="480060"/>
+          <a:ext cx="932957" cy="1043940"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>255824</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76320</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="圖片 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA37527B-5102-4978-8298-16E5EA1173E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2999024" y="449580"/>
+          <a:ext cx="917776" cy="1135380"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>486550</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>51737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>259079</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>144781</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="圖片 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A61DDB6D-D0DE-431B-B6CA-76B183A70E4A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4875670" y="432737"/>
+          <a:ext cx="869809" cy="1236044"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>126659</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>163197</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="圖片 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB6EAB63-C4FA-46FF-8D88-6A1DF14D8C0A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6545580" y="317159"/>
+          <a:ext cx="1569720" cy="1370038"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1794,10 +3766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244A819F-B465-4CC3-9D83-F08008DFAF0E}">
-  <dimension ref="A2:C2"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1817,6 +3789,30 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1826,10 +3822,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D7:Y29"/>
+  <dimension ref="D7:AC77"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G81" sqref="G81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -2386,10 +4382,782 @@
       <c r="X29" s="1"/>
       <c r="Y29" s="1"/>
     </row>
+    <row r="50" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1"/>
+      <c r="S50" s="1"/>
+      <c r="T50" s="1"/>
+      <c r="U50" s="1"/>
+      <c r="V50" s="1"/>
+      <c r="W50" s="1"/>
+      <c r="X50" s="1"/>
+      <c r="Y50" s="1"/>
+      <c r="Z50" s="1"/>
+      <c r="AA50" s="1"/>
+      <c r="AB50" s="1"/>
+      <c r="AC50" s="1"/>
+    </row>
+    <row r="51" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+      <c r="S51" s="1"/>
+      <c r="T51" s="1"/>
+      <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
+      <c r="W51" s="1"/>
+      <c r="X51" s="1"/>
+      <c r="Y51" s="1"/>
+      <c r="Z51" s="1"/>
+      <c r="AA51" s="1"/>
+      <c r="AB51" s="1"/>
+      <c r="AC51" s="1"/>
+    </row>
+    <row r="52" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
+      <c r="S52" s="1"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+      <c r="W52" s="1"/>
+      <c r="X52" s="1"/>
+      <c r="Y52" s="1"/>
+      <c r="Z52" s="1"/>
+      <c r="AA52" s="1"/>
+      <c r="AB52" s="1"/>
+      <c r="AC52" s="1"/>
+    </row>
+    <row r="53" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
+      <c r="S53" s="1"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
+      <c r="W53" s="1"/>
+      <c r="X53" s="1"/>
+      <c r="Y53" s="1"/>
+      <c r="Z53" s="1"/>
+      <c r="AA53" s="1"/>
+      <c r="AB53" s="1"/>
+      <c r="AC53" s="1"/>
+    </row>
+    <row r="54" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+      <c r="S54" s="1"/>
+      <c r="T54" s="1"/>
+      <c r="U54" s="1"/>
+      <c r="V54" s="1"/>
+      <c r="W54" s="1"/>
+      <c r="X54" s="1"/>
+      <c r="Y54" s="1"/>
+      <c r="Z54" s="1"/>
+      <c r="AA54" s="1"/>
+      <c r="AB54" s="1"/>
+      <c r="AC54" s="1"/>
+    </row>
+    <row r="55" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="1"/>
+      <c r="S55" s="1"/>
+      <c r="T55" s="1"/>
+      <c r="U55" s="1"/>
+      <c r="V55" s="1"/>
+      <c r="W55" s="1"/>
+      <c r="X55" s="1"/>
+      <c r="Y55" s="1"/>
+      <c r="Z55" s="1"/>
+      <c r="AA55" s="1"/>
+      <c r="AB55" s="1"/>
+      <c r="AC55" s="1"/>
+    </row>
+    <row r="56" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
+      <c r="S56" s="1"/>
+      <c r="T56" s="1"/>
+      <c r="U56" s="1"/>
+      <c r="V56" s="1"/>
+      <c r="W56" s="1"/>
+      <c r="X56" s="1"/>
+      <c r="Y56" s="1"/>
+      <c r="Z56" s="1"/>
+      <c r="AA56" s="1"/>
+      <c r="AB56" s="1"/>
+      <c r="AC56" s="1"/>
+    </row>
+    <row r="57" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="1"/>
+      <c r="T57" s="1"/>
+      <c r="U57" s="1"/>
+      <c r="V57" s="1"/>
+      <c r="W57" s="1"/>
+      <c r="X57" s="1"/>
+      <c r="Y57" s="1"/>
+      <c r="Z57" s="1"/>
+      <c r="AA57" s="1"/>
+      <c r="AB57" s="1"/>
+      <c r="AC57" s="1"/>
+    </row>
+    <row r="58" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="1"/>
+      <c r="T58" s="1"/>
+      <c r="U58" s="1"/>
+      <c r="V58" s="1"/>
+      <c r="W58" s="1"/>
+      <c r="X58" s="1"/>
+      <c r="Y58" s="1"/>
+      <c r="Z58" s="1"/>
+      <c r="AA58" s="1"/>
+      <c r="AB58" s="1"/>
+      <c r="AC58" s="1"/>
+    </row>
+    <row r="59" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
+      <c r="S59" s="1"/>
+      <c r="T59" s="1"/>
+      <c r="U59" s="1"/>
+      <c r="V59" s="1"/>
+      <c r="W59" s="1"/>
+      <c r="X59" s="1"/>
+      <c r="Y59" s="1"/>
+      <c r="Z59" s="1"/>
+      <c r="AA59" s="1"/>
+      <c r="AB59" s="1"/>
+      <c r="AC59" s="1"/>
+    </row>
+    <row r="60" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+      <c r="S60" s="1"/>
+      <c r="T60" s="1"/>
+      <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
+      <c r="W60" s="1"/>
+      <c r="X60" s="1"/>
+      <c r="Y60" s="1"/>
+      <c r="Z60" s="1"/>
+      <c r="AA60" s="1"/>
+      <c r="AB60" s="1"/>
+      <c r="AC60" s="1"/>
+    </row>
+    <row r="61" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="1"/>
+      <c r="S61" s="1"/>
+      <c r="T61" s="1"/>
+      <c r="U61" s="1"/>
+      <c r="V61" s="1"/>
+      <c r="W61" s="1"/>
+      <c r="X61" s="1"/>
+      <c r="Y61" s="1"/>
+      <c r="Z61" s="1"/>
+      <c r="AA61" s="1"/>
+      <c r="AB61" s="1"/>
+      <c r="AC61" s="1"/>
+    </row>
+    <row r="62" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="1"/>
+      <c r="S62" s="1"/>
+      <c r="T62" s="1"/>
+      <c r="U62" s="1"/>
+      <c r="V62" s="1"/>
+      <c r="W62" s="1"/>
+      <c r="X62" s="1"/>
+      <c r="Y62" s="1"/>
+      <c r="Z62" s="1"/>
+      <c r="AA62" s="1"/>
+      <c r="AB62" s="1"/>
+      <c r="AC62" s="1"/>
+    </row>
+    <row r="63" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1"/>
+      <c r="S63" s="1"/>
+      <c r="T63" s="1"/>
+      <c r="U63" s="1"/>
+      <c r="V63" s="1"/>
+      <c r="W63" s="1"/>
+      <c r="X63" s="1"/>
+      <c r="Y63" s="1"/>
+      <c r="Z63" s="1"/>
+      <c r="AA63" s="1"/>
+      <c r="AB63" s="1"/>
+      <c r="AC63" s="1"/>
+    </row>
+    <row r="64" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="1"/>
+      <c r="S64" s="1"/>
+      <c r="T64" s="1"/>
+      <c r="U64" s="1"/>
+      <c r="V64" s="1"/>
+      <c r="W64" s="1"/>
+      <c r="X64" s="1"/>
+      <c r="Y64" s="1"/>
+      <c r="Z64" s="1"/>
+      <c r="AA64" s="1"/>
+      <c r="AB64" s="1"/>
+      <c r="AC64" s="1"/>
+    </row>
+    <row r="65" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1"/>
+      <c r="S65" s="1"/>
+      <c r="T65" s="1"/>
+      <c r="U65" s="1"/>
+      <c r="V65" s="1"/>
+      <c r="W65" s="1"/>
+      <c r="X65" s="1"/>
+      <c r="Y65" s="1"/>
+      <c r="Z65" s="1"/>
+      <c r="AA65" s="1"/>
+      <c r="AB65" s="1"/>
+      <c r="AC65" s="1"/>
+    </row>
+    <row r="66" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="1"/>
+      <c r="S66" s="1"/>
+      <c r="T66" s="1"/>
+      <c r="U66" s="1"/>
+      <c r="V66" s="1"/>
+      <c r="W66" s="1"/>
+      <c r="X66" s="1"/>
+      <c r="Y66" s="1"/>
+      <c r="Z66" s="1"/>
+      <c r="AA66" s="1"/>
+      <c r="AB66" s="1"/>
+      <c r="AC66" s="1"/>
+    </row>
+    <row r="67" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1"/>
+      <c r="S67" s="1"/>
+      <c r="T67" s="1"/>
+      <c r="U67" s="1"/>
+      <c r="V67" s="1"/>
+      <c r="W67" s="1"/>
+      <c r="X67" s="1"/>
+      <c r="Y67" s="1"/>
+      <c r="Z67" s="1"/>
+      <c r="AA67" s="1"/>
+      <c r="AB67" s="1"/>
+      <c r="AC67" s="1"/>
+    </row>
+    <row r="68" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+      <c r="S68" s="1"/>
+      <c r="T68" s="1"/>
+      <c r="U68" s="1"/>
+      <c r="V68" s="1"/>
+      <c r="W68" s="1"/>
+      <c r="X68" s="1"/>
+      <c r="Y68" s="1"/>
+      <c r="Z68" s="1"/>
+      <c r="AA68" s="1"/>
+      <c r="AB68" s="1"/>
+      <c r="AC68" s="1"/>
+    </row>
+    <row r="69" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="1"/>
+      <c r="S69" s="1"/>
+      <c r="T69" s="1"/>
+      <c r="U69" s="1"/>
+      <c r="V69" s="1"/>
+      <c r="W69" s="1"/>
+      <c r="X69" s="1"/>
+      <c r="Y69" s="1"/>
+      <c r="Z69" s="1"/>
+      <c r="AA69" s="1"/>
+      <c r="AB69" s="1"/>
+      <c r="AC69" s="1"/>
+    </row>
+    <row r="70" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+      <c r="S70" s="1"/>
+      <c r="T70" s="1"/>
+      <c r="U70" s="1"/>
+      <c r="V70" s="1"/>
+      <c r="W70" s="1"/>
+      <c r="X70" s="1"/>
+      <c r="Y70" s="1"/>
+      <c r="Z70" s="1"/>
+      <c r="AA70" s="1"/>
+      <c r="AB70" s="1"/>
+      <c r="AC70" s="1"/>
+    </row>
+    <row r="71" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="1"/>
+      <c r="S71" s="1"/>
+      <c r="T71" s="1"/>
+      <c r="U71" s="1"/>
+      <c r="V71" s="1"/>
+      <c r="W71" s="1"/>
+      <c r="X71" s="1"/>
+      <c r="Y71" s="1"/>
+      <c r="Z71" s="1"/>
+      <c r="AA71" s="1"/>
+      <c r="AB71" s="1"/>
+      <c r="AC71" s="1"/>
+    </row>
+    <row r="72" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="1"/>
+      <c r="M72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="O72" s="1"/>
+      <c r="P72" s="1"/>
+      <c r="Q72" s="1"/>
+      <c r="R72" s="1"/>
+      <c r="S72" s="1"/>
+      <c r="T72" s="1"/>
+      <c r="U72" s="1"/>
+      <c r="V72" s="1"/>
+      <c r="W72" s="1"/>
+      <c r="X72" s="1"/>
+      <c r="Y72" s="1"/>
+      <c r="Z72" s="1"/>
+      <c r="AA72" s="1"/>
+      <c r="AB72" s="1"/>
+      <c r="AC72" s="1"/>
+    </row>
+    <row r="73" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
+      <c r="O73" s="1"/>
+      <c r="P73" s="1"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="1"/>
+      <c r="S73" s="1"/>
+      <c r="T73" s="1"/>
+      <c r="U73" s="1"/>
+      <c r="V73" s="1"/>
+      <c r="W73" s="1"/>
+      <c r="X73" s="1"/>
+      <c r="Y73" s="1"/>
+      <c r="Z73" s="1"/>
+      <c r="AA73" s="1"/>
+      <c r="AB73" s="1"/>
+      <c r="AC73" s="1"/>
+    </row>
+    <row r="74" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1"/>
+      <c r="O74" s="1"/>
+      <c r="P74" s="1"/>
+      <c r="Q74" s="1"/>
+      <c r="R74" s="1"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="1"/>
+      <c r="U74" s="1"/>
+      <c r="V74" s="1"/>
+      <c r="W74" s="1"/>
+      <c r="X74" s="1"/>
+      <c r="Y74" s="1"/>
+      <c r="Z74" s="1"/>
+      <c r="AA74" s="1"/>
+      <c r="AB74" s="1"/>
+      <c r="AC74" s="1"/>
+    </row>
+    <row r="75" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="1"/>
+      <c r="P75" s="1"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="1"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="1"/>
+      <c r="U75" s="1"/>
+      <c r="V75" s="1"/>
+      <c r="W75" s="1"/>
+      <c r="X75" s="1"/>
+      <c r="Y75" s="1"/>
+      <c r="Z75" s="1"/>
+      <c r="AA75" s="1"/>
+      <c r="AB75" s="1"/>
+      <c r="AC75" s="1"/>
+    </row>
+    <row r="76" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1"/>
+      <c r="L76" s="1"/>
+      <c r="M76" s="1"/>
+      <c r="N76" s="1"/>
+      <c r="O76" s="1"/>
+      <c r="P76" s="1"/>
+      <c r="Q76" s="1"/>
+      <c r="R76" s="1"/>
+      <c r="S76" s="1"/>
+      <c r="T76" s="1"/>
+      <c r="U76" s="1"/>
+      <c r="V76" s="1"/>
+      <c r="W76" s="1"/>
+      <c r="X76" s="1"/>
+      <c r="Y76" s="1"/>
+      <c r="Z76" s="1"/>
+      <c r="AA76" s="1"/>
+      <c r="AB76" s="1"/>
+      <c r="AC76" s="1"/>
+    </row>
+    <row r="77" spans="5:29" x14ac:dyDescent="0.3">
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+      <c r="L77" s="1"/>
+      <c r="M77" s="1"/>
+      <c r="N77" s="1"/>
+      <c r="O77" s="1"/>
+      <c r="P77" s="1"/>
+      <c r="Q77" s="1"/>
+      <c r="R77" s="1"/>
+      <c r="S77" s="1"/>
+      <c r="T77" s="1"/>
+      <c r="U77" s="1"/>
+      <c r="V77" s="1"/>
+      <c r="W77" s="1"/>
+      <c r="X77" s="1"/>
+      <c r="Y77" s="1"/>
+      <c r="Z77" s="1"/>
+      <c r="AA77" s="1"/>
+      <c r="AB77" s="1"/>
+      <c r="AC77" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEBB5A0C-2AA4-4446-9FDD-A45DF565FF82}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>